<commit_message>
Fixed Formatting Signed-off-by: ffpoke <aleard1@proton.me>
</commit_message>
<xml_diff>
--- a/2.x/2.5.xlsx
+++ b/2.x/2.5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marink\Documents\FFXIV Excel\2.x\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marink\Documents\FFXIV-EXCEL\2.x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E427E41B-3E5E-4057-82E9-4E887BDEBD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1EB507-0CBB-434E-993F-B17FA2F8B05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2.5" sheetId="2" r:id="rId1"/>
@@ -234,7 +234,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <extLst>
@@ -252,21 +252,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -632,9 +643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE1AAB13-9187-47F3-923D-0FEB0E4F4F54}">
   <dimension ref="B1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:H3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -817,9 +826,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B56C116-6BB5-4682-BFA7-37EE237ED682}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9:E13"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,32 +837,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="8" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
       <c r="E3">
         <v>10</v>
       </c>
@@ -862,11 +871,11 @@
       <c r="A4" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
       <c r="E4">
         <v>14</v>
       </c>
@@ -875,11 +884,11 @@
       <c r="A5" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
       <c r="E5">
         <v>14</v>
       </c>
@@ -888,11 +897,11 @@
       <c r="A6" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
       <c r="E6">
         <v>16</v>
       </c>
@@ -901,11 +910,11 @@
       <c r="A7" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
       <c r="E7">
         <v>8</v>
       </c>
@@ -914,11 +923,11 @@
       <c r="A8" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
       <c r="E8">
         <v>16</v>
       </c>
@@ -927,38 +936,38 @@
       <c r="A9" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="B11:E12"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="B11:E12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3:D3" r:id="rId1" location="'2.1 MSQ'!A1" display="A Realm Awoken (2.1)" xr:uid="{A3B218EB-4670-4FFE-A76C-45F76E81CC6D}"/>
@@ -978,7 +987,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,32 +996,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
       <c r="E1" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
       <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
       <c r="E3">
         <v>50</v>
       </c>
@@ -1021,11 +1030,11 @@
       <c r="A4" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
       <c r="E4">
         <v>50</v>
       </c>
@@ -1034,11 +1043,11 @@
       <c r="A5" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
       <c r="E5">
         <v>50</v>
       </c>
@@ -1047,11 +1056,11 @@
       <c r="A6" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
       <c r="E6">
         <v>50</v>
       </c>
@@ -1060,11 +1069,11 @@
       <c r="A7" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
       <c r="E7">
         <v>50</v>
       </c>
@@ -1073,11 +1082,11 @@
       <c r="A8" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
       <c r="E8">
         <v>50</v>
       </c>
@@ -1086,11 +1095,11 @@
       <c r="A9" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
       <c r="E9">
         <v>50</v>
       </c>
@@ -1099,27 +1108,27 @@
       <c r="A10" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
       <c r="E10">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="A1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="A1:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1127,10 +1136,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584A9A85-704A-474B-A729-F8B31BBED7C0}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,155 +1148,261 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
       <c r="E1" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
       <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="12" t="s">
         <v>20</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="12" t="s">
         <v>21</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="12" t="s">
         <v>22</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="12" t="s">
         <v>23</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6">
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="12" t="s">
         <v>24</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="12" t="s">
         <v>25</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="12" t="s">
         <v>26</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9">
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="12" t="s">
         <v>27</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10">
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="12" t="s">
         <v>28</v>
       </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11">
+        <v>50</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="A12" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>29</v>
       </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
+      <c r="A13" s="11"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13">
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B14" t="s">
-        <v>31</v>
+      <c r="B14" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B15" t="s">
-        <v>32</v>
+      <c r="B15" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15">
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B19" s="12" t="s">
         <v>35</v>
       </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="19">
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="E1:E2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>